<commit_message>
Latest changes pushed on 08-02-2026
</commit_message>
<xml_diff>
--- a/GroceryApplication/src/test/resources/testdatasample.xlsx
+++ b/GroceryApplication/src/test/resources/testdatasample.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jebin\eclipse-workspace\GroceryApplication\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jebin\git\SeleniumTestng\GroceryApplication\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E26A9D-CF4B-4AA8-92F4-8A72237ADE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B320F8F3-2B2D-4F43-98B8-EB45602092DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E5375BF0-41F4-4FD3-BD6B-CD153AEBDDA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{E5375BF0-41F4-4FD3-BD6B-CD153AEBDDA0}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageU" sheetId="1" r:id="rId1"/>
     <sheet name="AdminUsers" sheetId="2" r:id="rId2"/>
     <sheet name="ManageContact" sheetId="3" r:id="rId3"/>
     <sheet name="ManageFooter" sheetId="4" r:id="rId4"/>
+    <sheet name="ManageNews" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -78,7 +79,19 @@
     <t>testuserr@gmail.com</t>
   </si>
   <si>
-    <t>user27</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>user28</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Welcome</t>
   </si>
 </sst>
 </file>
@@ -500,10 +513,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157B0505-6A4D-4429-91DC-F3690A6D64B9}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,23 +525,29 @@
     <col min="2" max="2" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -622,4 +641,32 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F18AC87-D39E-479E-B6C0-5E732F05DB4E}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>